<commit_message>
iti bug fixed. itis changed
</commit_message>
<xml_diff>
--- a/iti_randomization.xlsx
+++ b/iti_randomization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Documents\GUESS\Guess_fMRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\Guess_fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD09DF53-FB48-4E3F-AD3E-717BBA503648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A85B01A-D71D-455D-91F6-7B2F810E35BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6B42273-C89E-401B-BEA5-DC942271AE65}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{B6B42273-C89E-401B-BEA5-DC942271AE65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -107,9 +107,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -147,7 +147,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -253,7 +253,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -405,216 +405,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BA7CCC-2BF3-4AC0-914E-5571BAB9284E}">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9</v>
       </c>

</xml_diff>